<commit_message>
mencoba membuat auth login, dengan 3 user, menyesuaikan import excel sesuai permintaan, dan memperbaiki tampilan tabel
</commit_message>
<xml_diff>
--- a/public/EmployeeData/managementdata.xlsx
+++ b/public/EmployeeData/managementdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thoriq\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40B4DA7-27E8-4E03-BC97-B9D59B1FF129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E0AC4C-FE74-45FF-B747-C12321B8B678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BDA41D0-06AA-4AA7-BC27-AE127E27DF33}"/>
   </bookViews>
@@ -25,21 +25,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>Banjarmasin</t>
   </si>
   <si>
-    <t>Banjarbaru</t>
-  </si>
-  <si>
-    <t>ATK</t>
+    <t>Alat Tulis Kantor</t>
+  </si>
+  <si>
+    <t>Alat tulis</t>
+  </si>
+  <si>
+    <t>Ballpoint 123</t>
+  </si>
+  <si>
+    <t>Buah</t>
+  </si>
+  <si>
+    <t>Faster</t>
+  </si>
+  <si>
+    <t>Spidol white board isi 12</t>
+  </si>
+  <si>
+    <t>Snowman</t>
+  </si>
+  <si>
+    <t>Ballpoint</t>
+  </si>
+  <si>
+    <t>Snowman V3</t>
+  </si>
+  <si>
+    <t>Snowman V2</t>
+  </si>
+  <si>
+    <t>Snowman V1</t>
+  </si>
+  <si>
+    <t>boxy unibal</t>
+  </si>
+  <si>
+    <t>Pilot G2</t>
+  </si>
+  <si>
+    <t>Tip ex</t>
+  </si>
+  <si>
+    <t>Re-Type</t>
+  </si>
+  <si>
+    <t>penghapus papan tulis</t>
+  </si>
+  <si>
+    <t>Cutter</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>Lem stik</t>
+  </si>
+  <si>
+    <t>kenko Kecil</t>
+  </si>
+  <si>
+    <t>kenko Besar</t>
+  </si>
+  <si>
+    <t>Bahan Kertas Dan Plastik</t>
+  </si>
+  <si>
+    <t>HVS Folio 70 Gram</t>
+  </si>
+  <si>
+    <t>Rim</t>
+  </si>
+  <si>
+    <t>Kiky</t>
+  </si>
+  <si>
+    <t>Bola Dunia</t>
+  </si>
+  <si>
+    <t>Alat Kantor</t>
+  </si>
+  <si>
+    <t>Perabot Kantor</t>
+  </si>
+  <si>
+    <t>Sapu</t>
+  </si>
+  <si>
+    <t>Ayam</t>
+  </si>
+  <si>
+    <t>Penyegar Ruangan</t>
+  </si>
+  <si>
+    <t>Bay Fresh</t>
+  </si>
+  <si>
+    <t>Stella</t>
+  </si>
+  <si>
+    <t>Personal Komputer</t>
+  </si>
+  <si>
+    <t>Desktop &amp; All In One Computer Lenovo</t>
+  </si>
+  <si>
+    <t>LENOVO AIO 520 22IKU Intel Core i3-7020U</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Core i3-7020U</t>
+  </si>
+  <si>
+    <t>Core i3-1005G1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;Rp&quot;#,##0;[Red]\-&quot;Rp&quot;#,##0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -57,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -65,12 +179,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,72 +517,449 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0147888C-6BD8-4165-B850-38AE31312716}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection sqref="A1:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>20000</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>20000</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>20000</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2023</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="3">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="3">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="3">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="3">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="3">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="3">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="3">
+        <v>7570000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="3">
+        <v>8001000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>